<commit_message>
Added maxmize, close, minimize btns
</commit_message>
<xml_diff>
--- a/PatientCare360/Excel/Users.xlsx
+++ b/PatientCare360/Excel/Users.xlsx
@@ -1,55 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dori6\source\repos\PatientCare360\PatientCare360\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A388559A-4225-4527-B60B-66EB00C497A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr autoCompressPictures="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Full name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>dori123</t>
-  </si>
-  <si>
-    <t>dori@123</t>
-  </si>
-  <si>
-    <t>316055656</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">316055656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123@$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315783522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori123%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori123#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,25 +91,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,16 +379,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -390,7 +410,53 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="default" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Register button, after you push it, it goes back into login form
</commit_message>
<xml_diff>
--- a/PatientCare360/Excel/Users.xlsx
+++ b/PatientCare360/Excel/Users.xlsx
@@ -1,55 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dori6\source\repos\PatientCare360\PatientCare360\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A388559A-4225-4527-B60B-66EB00C497A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr autoCompressPictures="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Full name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>dori123</t>
-  </si>
-  <si>
-    <t>dori@123</t>
-  </si>
-  <si>
-    <t>316055656</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dori@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">316055656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matan123@$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315783522</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,25 +79,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,16 +367,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -389,8 +397,32 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="default" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>